<commit_message>
Fix to classic defoliation and progress on iversen
</commit_message>
<xml_diff>
--- a/Prototypes/Chicory/ClassicObserved.xlsx
+++ b/Prototypes/Chicory/ClassicObserved.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
   <si>
     <t>Stage</t>
   </si>
@@ -35,19 +35,25 @@
     <t>Density</t>
   </si>
   <si>
-    <t>DMaccum</t>
-  </si>
-  <si>
     <t>SimulationName</t>
   </si>
   <si>
     <t>Classic</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>Above Ground Weight</t>
   </si>
   <si>
-    <t>Above Ground Weight</t>
+    <t>Chicory.AboveGround.Wt.kgha</t>
+  </si>
+  <si>
+    <t>Dmaccum.kgha</t>
+  </si>
+  <si>
+    <t>Dmaccum.gm2</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -2657,44 +2663,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="42.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" style="1" customWidth="1"/>
+    <col min="6" max="7" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2711,10 +2724,16 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2726,15 +2745,21 @@
         <v>6581.7</v>
       </c>
       <c r="E3">
+        <v>658.17</v>
+      </c>
+      <c r="F3">
+        <v>658.17</v>
+      </c>
+      <c r="G3">
         <v>6581.7</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>146.69999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2746,15 +2771,21 @@
         <v>2993.3</v>
       </c>
       <c r="E4">
+        <v>299.33000000000004</v>
+      </c>
+      <c r="F4">
+        <v>957.5</v>
+      </c>
+      <c r="G4">
         <v>9575</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2766,15 +2797,21 @@
         <v>3684</v>
       </c>
       <c r="E5">
+        <v>368.4</v>
+      </c>
+      <c r="F5">
+        <v>1325.9</v>
+      </c>
+      <c r="G5">
         <v>13259</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -2786,15 +2823,21 @@
         <v>1908</v>
       </c>
       <c r="E6">
+        <v>190.8</v>
+      </c>
+      <c r="F6">
+        <v>1516.7</v>
+      </c>
+      <c r="G6">
         <v>15167</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2806,15 +2849,21 @@
         <v>2075</v>
       </c>
       <c r="E7">
+        <v>207.5</v>
+      </c>
+      <c r="F7">
+        <v>207.5</v>
+      </c>
+      <c r="G7">
         <v>2075</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -2826,15 +2875,21 @@
         <v>2836</v>
       </c>
       <c r="E8">
+        <v>283.60000000000002</v>
+      </c>
+      <c r="F8">
+        <v>491.1</v>
+      </c>
+      <c r="G8">
         <v>4911</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -2846,15 +2901,21 @@
         <v>2616</v>
       </c>
       <c r="E9">
+        <v>261.60000000000002</v>
+      </c>
+      <c r="F9">
+        <v>752.7</v>
+      </c>
+      <c r="G9">
         <v>7527</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -2866,15 +2927,21 @@
         <v>923</v>
       </c>
       <c r="E10">
+        <v>92.3</v>
+      </c>
+      <c r="F10">
+        <v>845</v>
+      </c>
+      <c r="G10">
         <v>8450</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -2886,15 +2953,21 @@
         <v>617</v>
       </c>
       <c r="E11">
+        <v>61.7</v>
+      </c>
+      <c r="F11">
+        <v>906.7</v>
+      </c>
+      <c r="G11">
         <v>9067</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -2906,15 +2979,21 @@
         <v>1218</v>
       </c>
       <c r="E12">
+        <v>121.8</v>
+      </c>
+      <c r="F12">
+        <v>1028.5</v>
+      </c>
+      <c r="G12">
         <v>10285</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -2926,9 +3005,15 @@
         <v>1078</v>
       </c>
       <c r="E13">
+        <v>107.8</v>
+      </c>
+      <c r="F13">
+        <v>1136.3</v>
+      </c>
+      <c r="G13">
         <v>11363</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>14</v>
       </c>
     </row>

</xml_diff>